<commit_message>
updated messer score sheet
</commit_message>
<xml_diff>
--- a/static/beta/docs/Messer-Score-Sheet.xlsx
+++ b/static/beta/docs/Messer-Score-Sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9480" windowHeight="7005"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">Sue Orwin at sueorwin@btinternet.com </t>
   </si>
   <si>
-    <t>MESSER TROPHY 2018-2019</t>
+    <t>MESSER TROPHY 2019-2020</t>
   </si>
 </sst>
 </file>
@@ -683,7 +683,7 @@
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="B1" sqref="B1:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated messer draws etc.
</commit_message>
<xml_diff>
--- a/static/beta/docs/Messer-Score-Sheet.xlsx
+++ b/static/beta/docs/Messer-Score-Sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -122,32 +122,30 @@
     <t xml:space="preserve">Section A/B </t>
   </si>
   <si>
-    <t>One without the other won't count as a</t>
-  </si>
-  <si>
-    <t>receipt of the result.</t>
-  </si>
-  <si>
-    <t>by the winning team to the Messer Secretary,</t>
-  </si>
-  <si>
-    <t>This sheet should be filled in and emailed</t>
-  </si>
-  <si>
-    <t>with a scan/photo of the signed sheet.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sue Orwin at sueorwin@btinternet.com </t>
-  </si>
-  <si>
-    <t>MESSER TROPHY 2019-2020</t>
+    <t>MESSER TROPHY 2022-2023</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This sheet should be filled in and emailed by the winning team to the Messer Sceretary, Sue Orwin at stockportbadminton18@btinternet.com with a scan/photo of the signed sheet. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>One without the other won't count as a receipt of the result.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,15 +168,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,12 +179,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -282,26 +267,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -313,15 +288,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -329,7 +295,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T33"/>
+  <dimension ref="A1:X33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:P2"/>
+      <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,42 +667,42 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
+      <c r="B1" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
       <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
       <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -763,15 +729,15 @@
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="1"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -824,10 +790,10 @@
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="5"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -841,10 +807,10 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -861,10 +827,10 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -881,10 +847,10 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -907,79 +873,79 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="11" t="s">
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="8" t="s">
+      <c r="L11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="M11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N11" s="8" t="s">
+      <c r="N11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="O11" s="8" t="s">
+      <c r="O11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P11" s="12"/>
+      <c r="P11" s="10"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="12"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="10"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="12"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="10"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -989,17 +955,17 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="8"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="12"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="10"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -1015,138 +981,138 @@
         <v>29</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="12"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="10"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="5"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="4"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="5"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="12"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I16" s="6"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="10"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="8"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="12"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I17" s="6"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="10"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="8"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="12"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I18" s="6"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="10"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="8"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="12"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I19" s="6"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="10"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="8"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="12"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I20" s="6"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="10"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1155,12 +1121,12 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="4"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1175,7 +1141,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1193,16 +1159,16 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="6" t="s">
         <v>19</v>
       </c>
       <c r="H24" s="1"/>
@@ -1214,94 +1180,112 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13"/>
+      <c r="W24" s="13"/>
+      <c r="X24" s="13"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="24" t="s">
+      <c r="C25" s="4"/>
+      <c r="D25" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="25"/>
-      <c r="F25" s="16">
+      <c r="E25" s="18"/>
+      <c r="F25" s="12">
         <f>SUM(N12:N20)</f>
         <v>0</v>
       </c>
-      <c r="G25" s="15">
+      <c r="G25" s="11">
         <f>SUM(O12:O20)</f>
         <v>0</v>
       </c>
       <c r="H25" s="1"/>
-      <c r="I25" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="21"/>
-      <c r="O25" s="21"/>
+      <c r="I25" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
       <c r="P25" s="1"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="13"/>
+      <c r="W25" s="13"/>
+      <c r="X25" s="13"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="15">
+      <c r="E26" s="18"/>
+      <c r="F26" s="11">
         <f>SUM(J12:J20,L12:L17)</f>
         <v>0</v>
       </c>
-      <c r="G26" s="15">
+      <c r="G26" s="11">
         <f>SUM(K12:K20,M12:M17)</f>
         <v>0</v>
       </c>
       <c r="H26" s="1"/>
-      <c r="I26" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
       <c r="P26" s="1"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="13"/>
+      <c r="W26" s="13"/>
+      <c r="X26" s="13"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="4"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
       <c r="P27" s="1"/>
-      <c r="R27" s="26"/>
-      <c r="S27" s="26"/>
-      <c r="T27" s="26"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13"/>
+      <c r="W27" s="13"/>
+      <c r="X27" s="13"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1310,46 +1294,50 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="21"/>
-      <c r="O28" s="21"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
       <c r="P28" s="1"/>
-      <c r="R28" s="26"/>
-      <c r="S28" s="26"/>
-      <c r="T28" s="26"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="13"/>
+      <c r="W28" s="13"/>
+      <c r="X28" s="13"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="5"/>
+      <c r="C29" s="4"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
       <c r="P29" s="1"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="13"/>
+      <c r="W29" s="13"/>
+      <c r="X29" s="13"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1358,21 +1346,23 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-      <c r="I30" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="21"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
       <c r="P30" s="1"/>
-      <c r="R30" s="6"/>
-      <c r="S30" s="6"/>
-      <c r="T30" s="6"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
+      <c r="V30" s="13"/>
+      <c r="W30" s="13"/>
+      <c r="X30" s="13"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1381,19 +1371,23 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="R31" s="17"/>
-      <c r="S31" s="17"/>
-      <c r="T31" s="17"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="1"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="13"/>
+      <c r="W31" s="13"/>
+      <c r="X31" s="13"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1410,6 +1404,13 @@
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="13"/>
+      <c r="W32" s="13"/>
+      <c r="X32" s="13"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
@@ -1431,21 +1432,13 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="14">
-    <mergeCell ref="R31:T31"/>
+  <mergeCells count="6">
+    <mergeCell ref="I25:O31"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="B1:P2"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I25:O25"/>
-    <mergeCell ref="I26:O26"/>
-    <mergeCell ref="I27:O27"/>
-    <mergeCell ref="I28:O28"/>
-    <mergeCell ref="I29:O29"/>
-    <mergeCell ref="I30:O30"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D26:E26"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="R28:T28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>